<commit_message>
UI-829: Fixed IDs of tests
</commit_message>
<xml_diff>
--- a/design/Test Plan/TestPlan.xlsx
+++ b/design/Test Plan/TestPlan.xlsx
@@ -531,63 +531,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -652,6 +595,31 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -661,34 +629,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -697,6 +658,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1010,7 +1010,7 @@
   <dimension ref="B2:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1031,62 +1031,62 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="33"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="79"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="45"/>
+      <c r="C3" s="83"/>
       <c r="D3" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="47"/>
+      <c r="C4" s="85"/>
       <c r="D4" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="49"/>
+      <c r="C5" s="87"/>
       <c r="D5" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="50" t="s">
+      <c r="C6" s="81"/>
+      <c r="D6" s="31" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="2:12" s="3" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="37"/>
+      <c r="C7" s="81"/>
       <c r="D7" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="37"/>
+      <c r="C8" s="81"/>
       <c r="D8" s="9" t="s">
         <v>27</v>
       </c>
@@ -1109,7 +1109,7 @@
       <c r="C11" s="19">
         <v>1</v>
       </c>
-      <c r="D11" s="57" t="s">
+      <c r="D11" s="38" t="s">
         <v>58</v>
       </c>
       <c r="E11" s="21"/>
@@ -1117,33 +1117,33 @@
       <c r="G11" s="21"/>
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>
-      <c r="J11" s="58"/>
+      <c r="J11" s="39"/>
     </row>
     <row r="12" spans="2:12" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41" t="s">
+      <c r="E12" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="85" t="s">
+      <c r="F12" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="86"/>
-      <c r="H12" s="86"/>
-      <c r="I12" s="87"/>
-      <c r="J12" s="34" t="s">
+      <c r="G12" s="73"/>
+      <c r="H12" s="73"/>
+      <c r="I12" s="74"/>
+      <c r="J12" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="L12" s="84"/>
+      <c r="L12" s="61"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C13" s="35"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
       <c r="F13" s="10" t="s">
         <v>16</v>
       </c>
@@ -1156,11 +1156,11 @@
       <c r="I13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="35"/>
-      <c r="L13" s="84"/>
+      <c r="J13" s="76"/>
+      <c r="L13" s="61"/>
     </row>
     <row r="14" spans="2:12" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="C14" s="60" t="s">
+      <c r="C14" s="41" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="28" t="s">
@@ -1177,32 +1177,32 @@
       <c r="I14" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="J14" s="61"/>
-      <c r="L14" s="84"/>
+      <c r="J14" s="42"/>
+      <c r="L14" s="61"/>
     </row>
     <row r="15" spans="2:12" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="76" t="s">
+      <c r="C15" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="52" t="s">
+      <c r="D15" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="77" t="s">
+      <c r="E15" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="F15" s="53"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="I15" s="79" t="s">
-        <v>18</v>
-      </c>
-      <c r="J15" s="80"/>
-      <c r="L15" s="84"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="57"/>
+      <c r="L15" s="61"/>
     </row>
     <row r="16" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C16" s="60" t="s">
+      <c r="C16" s="41" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="28" t="s">
@@ -1219,28 +1219,28 @@
       <c r="I16" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="61"/>
-      <c r="L16" s="84"/>
+      <c r="J16" s="42"/>
+      <c r="L16" s="61"/>
     </row>
     <row r="17" spans="3:12" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="76" t="s">
+      <c r="C17" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="52" t="s">
+      <c r="D17" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="77" t="s">
+      <c r="E17" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="53"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="I17" s="79" t="s">
-        <v>18</v>
-      </c>
-      <c r="J17" s="80"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="57"/>
       <c r="L17"/>
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.3">
@@ -1249,12 +1249,12 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="62"/>
-      <c r="I18" s="62"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
       <c r="L18"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C19" s="63" t="s">
+      <c r="C19" s="44" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="4" t="s">
@@ -1265,49 +1265,49 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="64"/>
+      <c r="J19" s="45"/>
       <c r="L19"/>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C20" s="65">
-        <v>1</v>
-      </c>
-      <c r="D20" s="66" t="s">
+      <c r="C20" s="46">
+        <v>2</v>
+      </c>
+      <c r="D20" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="67"/>
-      <c r="F20" s="67"/>
-      <c r="G20" s="67"/>
-      <c r="H20" s="67"/>
-      <c r="I20" s="67"/>
-      <c r="J20" s="68"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="49"/>
       <c r="L20"/>
     </row>
     <row r="21" spans="3:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="41" t="s">
+      <c r="D21" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="41" t="s">
+      <c r="E21" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="85" t="s">
+      <c r="F21" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="86"/>
-      <c r="H21" s="86"/>
-      <c r="I21" s="87"/>
-      <c r="J21" s="41" t="s">
+      <c r="G21" s="73"/>
+      <c r="H21" s="73"/>
+      <c r="I21" s="74"/>
+      <c r="J21" s="67" t="s">
         <v>8</v>
       </c>
       <c r="L21"/>
     </row>
     <row r="22" spans="3:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="68"/>
       <c r="F22" s="10" t="s">
         <v>16</v>
       </c>
@@ -1320,10 +1320,10 @@
       <c r="I22" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="42"/>
+      <c r="J22" s="68"/>
     </row>
     <row r="23" spans="3:12" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="60" t="s">
+      <c r="C23" s="41" t="s">
         <v>11</v>
       </c>
       <c r="D23" s="26" t="s">
@@ -1340,30 +1340,30 @@
       <c r="I23" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="J23" s="61"/>
+      <c r="J23" s="42"/>
     </row>
     <row r="24" spans="3:12" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="76" t="s">
+      <c r="C24" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="51" t="s">
+      <c r="D24" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="52" t="s">
+      <c r="E24" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="53"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="I24" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="J24" s="80"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I24" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" s="57"/>
     </row>
     <row r="25" spans="3:12" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="69" t="s">
+      <c r="C25" s="50" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="27" t="s">
@@ -1380,30 +1380,30 @@
       <c r="I25" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="J25" s="70"/>
+      <c r="J25" s="51"/>
     </row>
     <row r="26" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C26" s="76" t="s">
+      <c r="C26" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="81" t="s">
+      <c r="D26" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="82" t="s">
+      <c r="E26" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="53"/>
-      <c r="G26" s="54"/>
-      <c r="H26" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="I26" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="J26" s="80"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I26" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="J26" s="57"/>
     </row>
     <row r="27" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C27" s="65" t="s">
+      <c r="C27" s="46" t="s">
         <v>41</v>
       </c>
       <c r="D27" s="30" t="s">
@@ -1420,30 +1420,30 @@
       <c r="I27" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J27" s="71"/>
+      <c r="J27" s="52"/>
     </row>
     <row r="28" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C28" s="76" t="s">
+      <c r="C28" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="82" t="s">
+      <c r="D28" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="82" t="s">
+      <c r="E28" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="F28" s="53"/>
-      <c r="G28" s="53"/>
-      <c r="H28" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="I28" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="J28" s="83"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I28" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="J28" s="60"/>
     </row>
     <row r="29" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C29" s="65" t="s">
+      <c r="C29" s="46" t="s">
         <v>47</v>
       </c>
       <c r="D29" s="30" t="s">
@@ -1460,7 +1460,7 @@
       <c r="I29" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J29" s="71"/>
+      <c r="J29" s="52"/>
     </row>
     <row r="30" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C30" s="2"/>
@@ -1468,11 +1468,11 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
-      <c r="H30" s="62"/>
-      <c r="I30" s="62"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="43"/>
     </row>
     <row r="31" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C31" s="63" t="s">
+      <c r="C31" s="44" t="s">
         <v>4</v>
       </c>
       <c r="D31" s="4" t="s">
@@ -1483,46 +1483,46 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
-      <c r="J31" s="64"/>
+      <c r="J31" s="45"/>
     </row>
     <row r="32" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C32" s="65">
-        <v>1</v>
-      </c>
-      <c r="D32" s="66" t="s">
+      <c r="C32" s="46">
+        <v>3</v>
+      </c>
+      <c r="D32" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="67"/>
-      <c r="F32" s="67"/>
-      <c r="G32" s="67"/>
-      <c r="H32" s="67"/>
-      <c r="I32" s="67"/>
-      <c r="J32" s="68"/>
+      <c r="E32" s="48"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="48"/>
+      <c r="H32" s="48"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="49"/>
     </row>
     <row r="33" spans="3:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="41" t="s">
+      <c r="C33" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="D33" s="41" t="s">
+      <c r="D33" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="41" t="s">
+      <c r="E33" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="F33" s="85" t="s">
+      <c r="F33" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="G33" s="86"/>
-      <c r="H33" s="86"/>
-      <c r="I33" s="87"/>
-      <c r="J33" s="41" t="s">
+      <c r="G33" s="73"/>
+      <c r="H33" s="73"/>
+      <c r="I33" s="74"/>
+      <c r="J33" s="67" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="34" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="68"/>
       <c r="F34" s="10" t="s">
         <v>16</v>
       </c>
@@ -1535,10 +1535,10 @@
       <c r="I34" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J34" s="42"/>
+      <c r="J34" s="68"/>
     </row>
     <row r="35" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C35" s="60" t="s">
+      <c r="C35" s="41" t="s">
         <v>11</v>
       </c>
       <c r="D35" s="28" t="s">
@@ -1555,28 +1555,28 @@
       <c r="I35" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="J35" s="61"/>
+      <c r="J35" s="42"/>
     </row>
     <row r="36" spans="3:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C36" s="76" t="s">
+      <c r="C36" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="D36" s="52" t="s">
+      <c r="D36" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="E36" s="77" t="s">
+      <c r="E36" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="F36" s="53"/>
-      <c r="G36" s="78"/>
-      <c r="H36" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="I36" s="79" t="s">
-        <v>18</v>
-      </c>
-      <c r="J36" s="80"/>
-      <c r="K36" s="59"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="55"/>
+      <c r="H36" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I36" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="J36" s="57"/>
+      <c r="K36" s="40"/>
     </row>
     <row r="37" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C37" s="2"/>
@@ -1584,11 +1584,11 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
-      <c r="H37" s="62"/>
-      <c r="I37" s="62"/>
+      <c r="H37" s="43"/>
+      <c r="I37" s="43"/>
     </row>
     <row r="38" spans="3:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="63" t="s">
+      <c r="C38" s="44" t="s">
         <v>4</v>
       </c>
       <c r="D38" s="4" t="s">
@@ -1599,46 +1599,46 @@
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
-      <c r="J38" s="64"/>
+      <c r="J38" s="45"/>
     </row>
     <row r="39" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C39" s="65">
-        <v>1</v>
-      </c>
-      <c r="D39" s="72" t="s">
+      <c r="C39" s="46">
+        <v>4</v>
+      </c>
+      <c r="D39" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="73"/>
-      <c r="F39" s="73"/>
-      <c r="G39" s="73"/>
-      <c r="H39" s="73"/>
-      <c r="I39" s="73"/>
-      <c r="J39" s="74"/>
+      <c r="E39" s="63"/>
+      <c r="F39" s="63"/>
+      <c r="G39" s="63"/>
+      <c r="H39" s="63"/>
+      <c r="I39" s="63"/>
+      <c r="J39" s="64"/>
     </row>
     <row r="40" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C40" s="38" t="s">
+      <c r="C40" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="D40" s="41" t="s">
+      <c r="D40" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="E40" s="40" t="s">
+      <c r="E40" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="F40" s="38" t="s">
+      <c r="F40" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="G40" s="39"/>
-      <c r="H40" s="39"/>
-      <c r="I40" s="40"/>
-      <c r="J40" s="41" t="s">
+      <c r="G40" s="71"/>
+      <c r="H40" s="71"/>
+      <c r="I40" s="69"/>
+      <c r="J40" s="67" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="41" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C41" s="75"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="43"/>
+      <c r="C41" s="66"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="70"/>
       <c r="F41" s="10" t="s">
         <v>16</v>
       </c>
@@ -1651,10 +1651,10 @@
       <c r="I41" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J41" s="42"/>
+      <c r="J41" s="68"/>
     </row>
     <row r="42" spans="3:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C42" s="60" t="s">
+      <c r="C42" s="41" t="s">
         <v>11</v>
       </c>
       <c r="D42" s="28" t="s">
@@ -1671,46 +1671,30 @@
       <c r="I42" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="J42" s="61"/>
+      <c r="J42" s="42"/>
     </row>
     <row r="43" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C43" s="76" t="s">
+      <c r="C43" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="D43" s="52" t="s">
+      <c r="D43" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="E43" s="77" t="s">
+      <c r="E43" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="F43" s="53"/>
-      <c r="G43" s="78"/>
-      <c r="H43" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="I43" s="79" t="s">
-        <v>18</v>
-      </c>
-      <c r="J43" s="80"/>
+      <c r="F43" s="34"/>
+      <c r="G43" s="55"/>
+      <c r="H43" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I43" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="J43" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="D39:J39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="J40:J41"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="J33:J34"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="J21:J22"/>
     <mergeCell ref="B6:C6"/>
@@ -1723,6 +1707,22 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D39:J39"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="J40:J41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
UI-888: UI-889: Added validation + highlighting row when user makes modifications to the webhook
</commit_message>
<xml_diff>
--- a/design/Test Plan/TestPlan.xlsx
+++ b/design/Test Plan/TestPlan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="67">
   <si>
     <t>Application Name</t>
   </si>
@@ -206,6 +206,15 @@
   </si>
   <si>
     <t>The banner appears on top, and shows some text describing what the Webhook app is.</t>
+  </si>
+  <si>
+    <t>Click on "Create" without typing any information</t>
+  </si>
+  <si>
+    <t>Error under name and URL, prompting the user to fill these fields</t>
+  </si>
+  <si>
+    <t>H</t>
   </si>
 </sst>
 </file>
@@ -441,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -480,16 +489,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -507,9 +510,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -519,31 +519,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -586,12 +574,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -610,9 +592,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -620,6 +599,60 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -635,12 +668,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -650,53 +677,62 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1007,10 +1043,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L43"/>
+  <dimension ref="B2:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1031,68 +1067,68 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="79"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="54"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="83"/>
+      <c r="C3" s="63"/>
       <c r="D3" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="85"/>
+      <c r="C4" s="65"/>
       <c r="D4" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="86" t="s">
+      <c r="B5" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="87"/>
+      <c r="C5" s="67"/>
       <c r="D5" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="80" t="s">
+      <c r="B6" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="81"/>
-      <c r="D6" s="31" t="s">
+      <c r="C6" s="58"/>
+      <c r="D6" s="26" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="2:12" s="3" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="80" t="s">
+      <c r="B7" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="81"/>
-      <c r="D7" s="18" t="s">
+      <c r="C7" s="58"/>
+      <c r="D7" s="16" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="81"/>
+      <c r="C8" s="58"/>
       <c r="D8" s="9" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="18" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -1106,44 +1142,44 @@
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="19">
+      <c r="C11" s="17">
         <v>1</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="39"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="32"/>
     </row>
     <row r="12" spans="2:12" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="75" t="s">
+      <c r="C12" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="67" t="s">
+      <c r="D12" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="67" t="s">
+      <c r="E12" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="72" t="s">
+      <c r="F12" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="73"/>
-      <c r="H12" s="73"/>
-      <c r="I12" s="74"/>
-      <c r="J12" s="75" t="s">
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="L12" s="61"/>
+      <c r="L12" s="51"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C13" s="76"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="68"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
       <c r="F13" s="10" t="s">
         <v>16</v>
       </c>
@@ -1156,14 +1192,14 @@
       <c r="I13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="76"/>
-      <c r="L13" s="61"/>
+      <c r="J13" s="69"/>
+      <c r="L13" s="51"/>
     </row>
     <row r="14" spans="2:12" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="24" t="s">
         <v>62</v>
       </c>
       <c r="E14" s="6" t="s">
@@ -1171,41 +1207,41 @@
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="13"/>
-      <c r="H14" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="I14" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J14" s="42"/>
-      <c r="L14" s="61"/>
+      <c r="H14" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="35"/>
+      <c r="L14" s="51"/>
     </row>
     <row r="15" spans="2:12" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="53" t="s">
+      <c r="C15" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="33" t="s">
+      <c r="D15" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="54" t="s">
+      <c r="E15" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="I15" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="J15" s="57"/>
-      <c r="L15" s="61"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="48"/>
+      <c r="L15" s="51"/>
     </row>
     <row r="16" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="24" t="s">
         <v>55</v>
       </c>
       <c r="E16" s="6" t="s">
@@ -1213,34 +1249,34 @@
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="13"/>
-      <c r="H16" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J16" s="42"/>
-      <c r="L16" s="61"/>
+      <c r="H16" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="35"/>
+      <c r="L16" s="51"/>
     </row>
     <row r="17" spans="3:12" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="53" t="s">
+      <c r="C17" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="54" t="s">
+      <c r="E17" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="34"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="I17" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="J17" s="57"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="48"/>
       <c r="L17"/>
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.3">
@@ -1249,12 +1285,12 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
       <c r="L18"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C19" s="44" t="s">
+      <c r="C19" s="37" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="4" t="s">
@@ -1265,49 +1301,49 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="45"/>
+      <c r="J19" s="38"/>
       <c r="L19"/>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C20" s="46">
+      <c r="C20" s="39">
         <v>2</v>
       </c>
-      <c r="D20" s="47" t="s">
+      <c r="D20" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48"/>
-      <c r="J20" s="49"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="42"/>
       <c r="L20"/>
     </row>
     <row r="21" spans="3:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="67" t="s">
+      <c r="C21" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="67" t="s">
+      <c r="D21" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="67" t="s">
+      <c r="E21" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="72" t="s">
+      <c r="F21" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="73"/>
-      <c r="H21" s="73"/>
-      <c r="I21" s="74"/>
-      <c r="J21" s="67" t="s">
+      <c r="G21" s="60"/>
+      <c r="H21" s="60"/>
+      <c r="I21" s="61"/>
+      <c r="J21" s="55" t="s">
         <v>8</v>
       </c>
       <c r="L21"/>
     </row>
     <row r="22" spans="3:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="56"/>
       <c r="F22" s="10" t="s">
         <v>16</v>
       </c>
@@ -1320,381 +1356,409 @@
       <c r="I22" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="68"/>
+      <c r="J22" s="56"/>
     </row>
     <row r="23" spans="3:12" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="41" t="s">
+      <c r="C23" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="D23" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E23" s="28" t="s">
+      <c r="E23" s="24" t="s">
         <v>23</v>
       </c>
       <c r="F23" s="12"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="I23" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J23" s="42"/>
-    </row>
-    <row r="24" spans="3:12" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="53" t="s">
+      <c r="G23" s="20"/>
+      <c r="H23" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="35"/>
+    </row>
+    <row r="24" spans="3:12" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="32" t="s">
+      <c r="D24" s="84" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="85" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" s="86"/>
+      <c r="G24" s="87"/>
+      <c r="H24" s="88"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="89"/>
+    </row>
+    <row r="25" spans="3:12" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="E25" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="34"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="I24" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="J24" s="57"/>
-    </row>
-    <row r="25" spans="3:12" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="27" t="s">
+      <c r="F25" s="21"/>
+      <c r="G25" s="80"/>
+      <c r="H25" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="I25" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J25" s="81"/>
+    </row>
+    <row r="26" spans="3:12" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="96" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="90" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="29" t="s">
+      <c r="E26" s="91" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="I25" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J25" s="51"/>
-    </row>
-    <row r="26" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C26" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="58" t="s">
+      <c r="F26" s="92"/>
+      <c r="G26" s="93"/>
+      <c r="H26" s="94" t="s">
+        <v>18</v>
+      </c>
+      <c r="I26" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="J26" s="95"/>
+    </row>
+    <row r="27" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C27" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="59" t="s">
+      <c r="E27" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="34"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="I26" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="J26" s="57"/>
-    </row>
-    <row r="27" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C27" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="30" t="s">
+      <c r="F27" s="21"/>
+      <c r="G27" s="80"/>
+      <c r="H27" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="I27" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="J27" s="81"/>
+    </row>
+    <row r="28" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C28" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="30" t="s">
+      <c r="E28" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="I27" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="J27" s="52"/>
-    </row>
-    <row r="28" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C28" s="53" t="s">
-        <v>44</v>
-      </c>
-      <c r="D28" s="59" t="s">
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="I28" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="J28" s="50"/>
+    </row>
+    <row r="29" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C29" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="59" t="s">
+      <c r="E29" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="I28" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="J28" s="60"/>
-    </row>
-    <row r="29" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C29" s="46" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="30" t="s">
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="I29" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="J29" s="43"/>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C30" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="E29" s="30" t="s">
+      <c r="E30" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="I29" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="J29" s="52"/>
-    </row>
-    <row r="30" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="43"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="I30" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="J30" s="50"/>
     </row>
     <row r="31" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C31" s="44" t="s">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="36"/>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C32" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="45"/>
-    </row>
-    <row r="32" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C32" s="46">
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="38"/>
+    </row>
+    <row r="33" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C33" s="39">
         <v>3</v>
       </c>
-      <c r="D32" s="47" t="s">
+      <c r="D33" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="48"/>
-      <c r="H32" s="48"/>
-      <c r="I32" s="48"/>
-      <c r="J32" s="49"/>
-    </row>
-    <row r="33" spans="3:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="67" t="s">
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="41"/>
+      <c r="J33" s="42"/>
+    </row>
+    <row r="34" spans="3:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="D33" s="67" t="s">
+      <c r="D34" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="67" t="s">
+      <c r="E34" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="F33" s="72" t="s">
+      <c r="F34" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="G33" s="73"/>
-      <c r="H33" s="73"/>
-      <c r="I33" s="74"/>
-      <c r="J33" s="67" t="s">
+      <c r="G34" s="60"/>
+      <c r="H34" s="60"/>
+      <c r="I34" s="61"/>
+      <c r="J34" s="55" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C34" s="68"/>
-      <c r="D34" s="68"/>
-      <c r="E34" s="68"/>
-      <c r="F34" s="10" t="s">
+    <row r="35" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C35" s="56"/>
+      <c r="D35" s="56"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G34" s="11" t="s">
+      <c r="G35" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H34" s="10" t="s">
+      <c r="H35" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="I34" s="10" t="s">
+      <c r="I35" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J34" s="68"/>
-    </row>
-    <row r="35" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C35" s="41" t="s">
+      <c r="J35" s="56"/>
+    </row>
+    <row r="36" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C36" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="28" t="s">
+      <c r="D36" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="E36" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F35" s="12"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="I35" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J35" s="42"/>
-    </row>
-    <row r="36" spans="3:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C36" s="53" t="s">
+      <c r="F36" s="12"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I36" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J36" s="35"/>
+    </row>
+    <row r="37" spans="3:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C37" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="D36" s="33" t="s">
+      <c r="D37" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="E36" s="54" t="s">
+      <c r="E37" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="F36" s="34"/>
-      <c r="G36" s="55"/>
-      <c r="H36" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="I36" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="J36" s="57"/>
-      <c r="K36" s="40"/>
-    </row>
-    <row r="37" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="43"/>
-    </row>
-    <row r="38" spans="3:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="44" t="s">
+      <c r="F37" s="28"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="J37" s="48"/>
+      <c r="K37" s="33"/>
+    </row>
+    <row r="38" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+    </row>
+    <row r="39" spans="3:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D39" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="45"/>
-    </row>
-    <row r="39" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C39" s="46">
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="38"/>
+    </row>
+    <row r="40" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C40" s="39">
         <v>4</v>
       </c>
-      <c r="D39" s="62" t="s">
+      <c r="D40" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="63"/>
-      <c r="F39" s="63"/>
-      <c r="G39" s="63"/>
-      <c r="H39" s="63"/>
-      <c r="I39" s="63"/>
-      <c r="J39" s="64"/>
-    </row>
-    <row r="40" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C40" s="65" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" s="67" t="s">
-        <v>6</v>
-      </c>
-      <c r="E40" s="69" t="s">
-        <v>7</v>
-      </c>
-      <c r="F40" s="65" t="s">
-        <v>15</v>
-      </c>
+      <c r="E40" s="71"/>
+      <c r="F40" s="71"/>
       <c r="G40" s="71"/>
       <c r="H40" s="71"/>
-      <c r="I40" s="69"/>
-      <c r="J40" s="67" t="s">
+      <c r="I40" s="71"/>
+      <c r="J40" s="72"/>
+    </row>
+    <row r="41" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C41" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="55" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="75" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="73" t="s">
+        <v>15</v>
+      </c>
+      <c r="G41" s="77"/>
+      <c r="H41" s="77"/>
+      <c r="I41" s="75"/>
+      <c r="J41" s="55" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C41" s="66"/>
-      <c r="D41" s="68"/>
-      <c r="E41" s="70"/>
-      <c r="F41" s="10" t="s">
+    <row r="42" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C42" s="74"/>
+      <c r="D42" s="56"/>
+      <c r="E42" s="76"/>
+      <c r="F42" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G41" s="11" t="s">
+      <c r="G42" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H41" s="10" t="s">
+      <c r="H42" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="I41" s="10" t="s">
+      <c r="I42" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J41" s="68"/>
-    </row>
-    <row r="42" spans="3:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C42" s="41" t="s">
+      <c r="J42" s="56"/>
+    </row>
+    <row r="43" spans="3:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C43" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="D42" s="28" t="s">
+      <c r="D43" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="E43" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F42" s="12"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="I42" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J42" s="42"/>
-    </row>
-    <row r="43" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C43" s="53" t="s">
+      <c r="F43" s="12"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I43" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J43" s="35"/>
+    </row>
+    <row r="44" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C44" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="D43" s="33" t="s">
+      <c r="D44" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E43" s="54" t="s">
+      <c r="E44" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="F43" s="34"/>
-      <c r="G43" s="55"/>
-      <c r="H43" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="I43" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="J43" s="57"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="46"/>
+      <c r="H44" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="I44" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="J44" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D40:J40"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="J41:J42"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="J34:J35"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="J21:J22"/>
     <mergeCell ref="B6:C6"/>
@@ -1707,22 +1771,10 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="J33:J34"/>
     <mergeCell ref="F12:I12"/>
     <mergeCell ref="J12:J13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D39:J39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="J40:J41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>